<commit_message>
solved empy table error
</commit_message>
<xml_diff>
--- a/notas_colaboradores.xlsx
+++ b/notas_colaboradores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FranciscoFontoura\Documents\projects\franciscofontoura.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAE3271-BA9C-4CA8-8638-49441256CBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE840F9-0B1C-42AD-BDFE-E2588ED3CFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{82CD1E30-E8F4-44D7-9F7D-D89F3547E0EA}"/>
   </bookViews>
@@ -220,7 +220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,33 +237,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -308,23 +286,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,35 +301,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -678,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4420DBD1-D975-456A-9843-8CC5E343D9E2}">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,1135 +643,598 @@
     <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="7">
         <v>21998764554</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="7">
         <v>21978965744</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="14"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="7">
         <v>21987773833</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="7">
         <v>21997657410</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="7">
         <v>21999907633</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="13" t="s">
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="7">
         <v>21992926643</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="7">
         <v>21986881074</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="13" t="s">
+      <c r="G8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="7">
         <v>21988445709</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="13" t="s">
+      <c r="G9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="7">
         <v>21992100001</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="13" t="s">
+      <c r="F10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="14"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="7">
         <v>21987773833</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="14"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="H11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="7">
         <v>21983836666</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="13" t="s">
+      <c r="D12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="7">
         <v>21999990878</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="14"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="7">
         <v>21991927666</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="7">
         <v>21984847777</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="7">
         <v>21987773833</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="14"/>
+      <c r="G16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="7">
         <v>21999009766</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="14"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="7">
         <v>21992456372</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="13" t="s">
+      <c r="E18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="14"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="7">
         <v>21999281122</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="14"/>
+      <c r="H19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="7">
         <v>21987773833</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="14"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="7">
         <v>21995685881</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="J45" s="4"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
+      <c r="I21" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A22:A74">
-    <cfRule type="duplicateValues" dxfId="0" priority="21"/>
-  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2038,18 +1455,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9764725A-CCED-415E-BB23-5F17BF6D780F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B33DA284-65A8-4642-A9EA-3910EE30AE48}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B33DA284-65A8-4642-A9EA-3910EE30AE48}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9764725A-CCED-415E-BB23-5F17BF6D780F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>